<commit_message>
hoàn thành nốt crud
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,13 +8,18 @@
   </bookViews>
   <sheets>
     <sheet name="nội dung tranning" sheetId="1" r:id="rId1"/>
+    <sheet name="springdatajpa" sheetId="2" r:id="rId2"/>
+    <sheet name="Custom query" sheetId="3" r:id="rId3"/>
+    <sheet name="Page&amp;Sort&amp;Transation" sheetId="4" r:id="rId4"/>
+    <sheet name="Lombook&amp;DevTool" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet5" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve">Tìm hiểu các nội dung dưới(Trong 2 ngày):
 1. Khái niệm, mục đích sử dụng của Spring Data JPA
@@ -40,14 +45,79 @@
  1. Khái niệm, mục đích sử dụng của Thư viện ModelMapper trong Spring. Cho ví dụ chi tiết, cụ thể
  2. Khái niệm, mục đích sử dụng của Specification(Where) Spring Data JPA. cho ví dụ chi tiết, cụ thể</t>
   </si>
+  <si>
+    <t>Spring data jpa</t>
+  </si>
+  <si>
+    <t>Khái niệm</t>
+  </si>
+  <si>
+    <t>Spring Data JPA là một phần mềm của Spring Framework, cung cấp một cách tiếp cận đơn giản và tự động hóa việc truy vấn cơ sở dữ liệu quan hệ trong ứng dụng Java. Nó sử dụng Java Persistence API (JPA) để thực hiện các thao tác truy vấn cơ sở dữ liệu, giúp giảm thiểu việc viết mã SQL thủ công.</t>
+  </si>
+  <si>
+    <t>Mục đích</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mục đích của Spring Data JPA là đơn giản hóa việc truy vấn cơ sở dữ liệu và giúp cho các nhà phát triển tập trung vào việc phát triển các chức năng ứng dụng thay vì việc quản lý cơ sở dữ liệu và cú pháp truy vấn phức tạp. Spring Data JPA cung cấp một số tính năng như:
+- Tự động tạo câu truy vấn SQL dựa trên các phương thức của interface.
+- Hỗ trợ paging và sorting cho các kết quả truy vấn.
+- Cung cấp các phương thức mặc định để thực hiện các thao tác CRUD (create, read, update, delete).
+- Cho phép xử lý các quan hệ giữa các thực thể cơ sở dữ liệu một cách dễ dàng hơn.
+- Tích hợp với các tính năng khác của Spring Framework như Dependency Injection.
+</t>
+  </si>
+  <si>
+    <t>Custom query</t>
+  </si>
+  <si>
+    <t>Custom methods</t>
+  </si>
+  <si>
+    <t>@Query</t>
+  </si>
+  <si>
+    <t>để chỉ định các truy vấn tùy chỉnh (custom query) để truy xuất dữ liệu từ cơ sở dữ liệu. Custom query thường được sử dụng để tạo ra các truy vấn phức tạp, không thể đạt được bằng cách sử dụng các phương thức truy vấn cơ bản như findBy, findAll, ... trong Repository của Spring.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Các phương thức được định nghĩa trong Repository interface để thực hiện các truy vấn tùy chỉnh hoặc các thao tác khác với cơ sở dữ liệu. Custom Methods cho phép chúng ta định nghĩa các truy vấn tùy chỉnh mà không cần phải viết các truy vấn SQL hoặc JPQL.
+</t>
+  </si>
+  <si>
+    <t>@Query là một annotation trong Spring Data JPA cho phép định nghĩa các truy vấn tùy chỉnh dưới dạng câu truy vấn SQL. Các truy vấn này có thể được sử dụng để thực hiện các thao tác đọc/ghi dữ liệu vào cơ sở dữ liệu.</t>
+  </si>
+  <si>
+    <t>Page&amp;Sort</t>
+  </si>
+  <si>
+    <t>@Transaction</t>
+  </si>
+  <si>
+    <t>Paging và Sorting là hai tính năng quan trọng trong việc hiển thị dữ liệu trong ứng dụng web. Trong Spring Boot, có thể sử dụng Spring Data JPA để hỗ trợ việc phân trang và sắp xếp.</t>
+  </si>
+  <si>
+    <t>Trong Spring Boot, @Transactional là một annotation được sử dụng để quản lý transaction trong ứng dụng. Khi một method được đánh dấu với @Transactional, Spring Boot sẽ tạo ra một transaction để đảm bảo tính toàn vẹn dữ liệu.</t>
+  </si>
+  <si>
+    <t>Lombook</t>
+  </si>
+  <si>
+    <t>Devtool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lombok là một thư viện mã nguồn mở cho phép bạn giảm thiểu lượng mã boilerplate (mã lặp đi lặp lại) trong các project Java. Lombok cung cấp các annotation để tạo ra các method getter/setter, constructors, equals(), hashCode(), toString() và nhiều method khác với một cách nhanh chóng và đơn giản hơn.
+</t>
+  </si>
+  <si>
+    <t>Spring Boot DevTools là một module của Spring Boot cung cấp các tính năng hỗ trợ phát triển ứng dụng như tự động khởi động lại ứng dụng khi có sự thay đổi trong mã nguồn, reload trình duyệt, logging thực thi, v.v.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
@@ -61,19 +131,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -82,9 +152,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -106,18 +191,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -138,7 +223,7 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -161,7 +246,14 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -169,29 +261,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,31 +283,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -249,151 +463,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -404,6 +474,21 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -470,21 +555,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -509,7 +579,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -530,133 +600,139 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -720,6 +796,53 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>2438400</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="704850" y="1438275"/>
+          <a:ext cx="6191250" cy="952500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -983,7 +1106,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="1"/>
@@ -993,10 +1116,10 @@
   </cols>
   <sheetData>
     <row r="1" ht="300" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1004,4 +1127,198 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="10.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="86.1428571428571" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:2">
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" ht="60" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" ht="165" spans="1:2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="10.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="56.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="53" customWidth="1"/>
+    <col min="4" max="4" width="46" customWidth="1"/>
+    <col min="5" max="5" width="39.4285714285714" customWidth="1"/>
+    <col min="6" max="6" width="36.8571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" ht="90" spans="1:4">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="10.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="77" customWidth="1"/>
+    <col min="3" max="3" width="82.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" ht="45" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="10.4285714285714" customWidth="1"/>
+    <col min="2" max="2" width="64.4285714285714" customWidth="1"/>
+    <col min="3" max="3" width="64.5714285714286" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3">
+      <c r="B1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" ht="90" spans="1:3">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>